<commit_message>
In progress - BigHomeWork5
</commit_message>
<xml_diff>
--- a/BigHomeWork5/Matrica.xlsx
+++ b/BigHomeWork5/Matrica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C_Sharp\GitHub\BigHomeWork5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B79D6A-BEF1-46BB-B950-D46C7D661575}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0201435C-5096-4C45-8840-9F3D33AE68EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16935" yWindow="1845" windowWidth="15150" windowHeight="13695" xr2:uid="{2711DD60-25E4-4D42-9756-2F171D3D35B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2711DD60-25E4-4D42-9756-2F171D3D35B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Lapas1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>(1;4)</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>(24; 0)</t>
+  </si>
+  <si>
+    <t>(4; 1)</t>
+  </si>
+  <si>
+    <t>(5; 1)</t>
+  </si>
+  <si>
+    <t>(4; 2)</t>
+  </si>
+  <si>
+    <t>(5; 2)</t>
   </si>
 </sst>
 </file>
@@ -67,7 +79,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +101,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -120,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -129,6 +147,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
@@ -443,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C258D8-6C34-4A58-8345-2F6CC5536FF0}">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +474,7 @@
     <col min="2" max="18" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="6">
         <v>0</v>
       </c>
@@ -479,15 +498,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="2"/>
@@ -502,16 +521,34 @@
       <c r="R2" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" t="s">
+        <v>6</v>
+      </c>
+      <c r="W2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -526,8 +563,14 @@
       <c r="R3" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -553,7 +596,7 @@
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
     </row>
-    <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -583,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -609,7 +652,7 @@
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
     </row>
-    <row r="7" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -635,7 +678,7 @@
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
     </row>
-    <row r="8" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -661,7 +704,7 @@
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
     </row>
-    <row r="9" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -687,7 +730,7 @@
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
     </row>
-    <row r="10" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -713,7 +756,7 @@
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
     </row>
-    <row r="11" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -739,7 +782,7 @@
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
     </row>
-    <row r="12" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -765,7 +808,7 @@
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
     </row>
-    <row r="13" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -791,7 +834,7 @@
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
     </row>
-    <row r="14" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -817,7 +860,7 @@
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
     </row>
-    <row r="15" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -847,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
BigHomeWork - with Figures coordinates
</commit_message>
<xml_diff>
--- a/BigHomeWork5/Matrica.xlsx
+++ b/BigHomeWork5/Matrica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C_Sharp\GitHub\BigHomeWork5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0201435C-5096-4C45-8840-9F3D33AE68EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6962DD-6FAF-49D1-8AF7-B1BD86771123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2711DD60-25E4-4D42-9756-2F171D3D35B7}"/>
+    <workbookView xWindow="3945" yWindow="2610" windowWidth="20835" windowHeight="11385" xr2:uid="{2711DD60-25E4-4D42-9756-2F171D3D35B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Lapas1" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
-  <si>
-    <t>(1;4)</t>
-  </si>
-  <si>
-    <t>(4;1)</t>
-  </si>
-  <si>
-    <t>(15; 14)</t>
-  </si>
-  <si>
-    <t>(14; 15)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="27">
   <si>
     <t>(0;  24)</t>
   </si>
@@ -45,23 +33,86 @@
     <t>(24; 0)</t>
   </si>
   <si>
-    <t>(4; 1)</t>
-  </si>
-  <si>
-    <t>(5; 1)</t>
-  </si>
-  <si>
-    <t>(4; 2)</t>
-  </si>
-  <si>
-    <t>(5; 2)</t>
+    <t>C</t>
+  </si>
+  <si>
+    <t>0;0</t>
+  </si>
+  <si>
+    <t>(-1 ;-1)</t>
+  </si>
+  <si>
+    <t>(0; 0)</t>
+  </si>
+  <si>
+    <t>(1; -1)</t>
+  </si>
+  <si>
+    <t>(1; 1)</t>
+  </si>
+  <si>
+    <t>(-1; +1)</t>
+  </si>
+  <si>
+    <t>(+1; +1)</t>
+  </si>
+  <si>
+    <t>(-1; -1)</t>
+  </si>
+  <si>
+    <t>(+1; -1)</t>
+  </si>
+  <si>
+    <t>(+2; 0)</t>
+  </si>
+  <si>
+    <t>(+1; +2)</t>
+  </si>
+  <si>
+    <t>(-2; 0)</t>
+  </si>
+  <si>
+    <t>(0; -2)</t>
+  </si>
+  <si>
+    <t>(-1 ;0)</t>
+  </si>
+  <si>
+    <t>(+1; 0)</t>
+  </si>
+  <si>
+    <t>(0; -1)</t>
+  </si>
+  <si>
+    <t>(0; +1)</t>
+  </si>
+  <si>
+    <t>(0; +2)</t>
+  </si>
+  <si>
+    <t>(-1;  0)</t>
+  </si>
+  <si>
+    <t>(0 ;-1)</t>
+  </si>
+  <si>
+    <t>(-1; 0)</t>
+  </si>
+  <si>
+    <t>(+1 ; 0)</t>
+  </si>
+  <si>
+    <t>(-1 ; 0)</t>
+  </si>
+  <si>
+    <t>(1; 0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,8 +129,17 @@
       <charset val="186"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,8 +170,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -134,11 +206,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -148,6 +246,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
@@ -462,19 +577,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C258D8-6C34-4A58-8345-2F6CC5536FF0}">
-  <dimension ref="A1:AC25"/>
+  <dimension ref="A1:AM63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="18" width="3.140625" customWidth="1"/>
+    <col min="20" max="20" width="4" customWidth="1"/>
+    <col min="21" max="21" width="4.28515625" customWidth="1"/>
+    <col min="22" max="23" width="5.5703125" customWidth="1"/>
+    <col min="25" max="26" width="6.5703125" customWidth="1"/>
+    <col min="27" max="27" width="5.42578125" customWidth="1"/>
+    <col min="28" max="28" width="4.85546875" customWidth="1"/>
+    <col min="29" max="29" width="5" customWidth="1"/>
+    <col min="30" max="30" width="5.5703125" customWidth="1"/>
+    <col min="31" max="31" width="6.5703125" customWidth="1"/>
+    <col min="32" max="32" width="5.140625" customWidth="1"/>
+    <col min="33" max="33" width="5.85546875" customWidth="1"/>
+    <col min="34" max="34" width="5.7109375" customWidth="1"/>
+    <col min="35" max="37" width="5.5703125" customWidth="1"/>
+    <col min="38" max="38" width="5.85546875" customWidth="1"/>
+    <col min="39" max="39" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="6">
         <v>0</v>
       </c>
@@ -498,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -506,10 +636,12 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="F2" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="2"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -521,26 +653,24 @@
       <c r="R2" s="7">
         <v>1</v>
       </c>
-      <c r="V2" t="s">
-        <v>6</v>
-      </c>
-      <c r="W2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="19">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="1"/>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -563,14 +693,32 @@
       <c r="R3" s="7">
         <v>1</v>
       </c>
-      <c r="V3" t="s">
-        <v>8</v>
-      </c>
-      <c r="W3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Y3" s="19">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="19">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="19">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="1"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="4"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="4">
+        <v>2</v>
+      </c>
+      <c r="AM3" s="1"/>
+    </row>
+    <row r="4" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -594,17 +742,35 @@
         <v>1</v>
       </c>
       <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-    </row>
-    <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="U4" s="16"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="4">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>4</v>
+      </c>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="1"/>
+    </row>
+    <row r="5" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -619,14 +785,14 @@
       <c r="R5" s="7">
         <v>1</v>
       </c>
-      <c r="T5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="T5" s="17"/>
+      <c r="U5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" s="18"/>
+      <c r="W5" s="4"/>
+    </row>
+    <row r="6" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -650,17 +816,34 @@
         <v>1</v>
       </c>
       <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-    </row>
-    <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="U6" s="16"/>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -676,15 +859,30 @@
         <v>1</v>
       </c>
       <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-    </row>
-    <row r="8" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="U7" s="16"/>
+      <c r="X7">
+        <v>2</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -703,8 +901,23 @@
       </c>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
-    </row>
-    <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="X8">
+        <v>3</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -712,7 +925,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="9"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -729,16 +942,33 @@
       </c>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
-    </row>
-    <row r="10" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="X9">
+        <v>4</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="14"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -755,8 +985,28 @@
       </c>
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
-    </row>
-    <row r="11" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="4">
+        <v>4</v>
+      </c>
+      <c r="AM10" s="1"/>
+    </row>
+    <row r="11" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -781,15 +1031,37 @@
       </c>
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
-    </row>
-    <row r="12" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="4">
+        <v>3</v>
+      </c>
+      <c r="AM11" s="1"/>
+    </row>
+    <row r="12" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="14" t="s">
+        <v>2</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -807,16 +1079,52 @@
       </c>
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
-    </row>
-    <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="X12" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="19">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="19">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="19">
+        <v>4</v>
+      </c>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="4">
+        <v>3</v>
+      </c>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="4">
+        <v>4</v>
+      </c>
+      <c r="AG12" s="4">
+        <v>3</v>
+      </c>
+      <c r="AH12" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI12" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="4">
+        <v>2</v>
+      </c>
+      <c r="AM12" s="1"/>
+    </row>
+    <row r="13" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -833,8 +1141,28 @@
       </c>
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
-    </row>
-    <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="4">
+        <v>4</v>
+      </c>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM13" s="1"/>
+    </row>
+    <row r="14" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -860,7 +1188,7 @@
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
     </row>
-    <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -868,8 +1196,8 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -879,26 +1207,39 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="4"/>
+      <c r="Q15" s="3"/>
       <c r="R15" s="7">
         <v>1</v>
       </c>
-      <c r="T15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="U15" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -915,8 +1256,23 @@
       </c>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
-    </row>
-    <row r="17" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="X16">
+        <v>2</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -941,13 +1297,28 @@
       </c>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
-    </row>
-    <row r="18" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="X17">
+        <v>3</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -967,15 +1338,32 @@
       </c>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X18">
+        <v>4</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="10"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -992,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -1015,8 +1403,39 @@
       <c r="R20" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="19">
+        <v>4</v>
+      </c>
+      <c r="AB20" s="21"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="4">
+        <v>4</v>
+      </c>
+      <c r="AF20" s="21"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI20" s="4">
+        <v>4</v>
+      </c>
+      <c r="AJ20" s="21"/>
+      <c r="AK20" s="3"/>
+      <c r="AL20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -1039,8 +1458,39 @@
       <c r="R21" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Y21" s="20"/>
+      <c r="Z21" s="19">
+        <v>2</v>
+      </c>
+      <c r="AA21" s="19">
+        <v>3</v>
+      </c>
+      <c r="AB21" s="21"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE21" s="4">
+        <v>3</v>
+      </c>
+      <c r="AF21" s="21"/>
+      <c r="AG21" s="3"/>
+      <c r="AH21" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI21" s="4">
+        <v>3</v>
+      </c>
+      <c r="AJ21" s="21"/>
+      <c r="AK21" s="3"/>
+      <c r="AL21" s="4">
+        <v>2</v>
+      </c>
+      <c r="AM21" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -1063,8 +1513,23 @@
       <c r="R22" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="21"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="21"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="21"/>
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="3"/>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -1088,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -1111,8 +1576,23 @@
       <c r="R24" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X24">
+        <v>1</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -1168,10 +1648,663 @@
         <v>17</v>
       </c>
       <c r="T25" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U25" t="s">
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <v>2</v>
+      </c>
+      <c r="Z25" t="s">
         <v>5</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="X26">
+        <v>3</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="X27">
+        <v>4</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="Y29" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA29" s="20"/>
+      <c r="AB29" s="21"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF29" s="21"/>
+      <c r="AG29" s="3"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="21"/>
+      <c r="AK29" s="3"/>
+      <c r="AL29" s="4">
+        <v>4</v>
+      </c>
+      <c r="AM29" s="3"/>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="Y30" s="20"/>
+      <c r="Z30" s="19">
+        <v>2</v>
+      </c>
+      <c r="AA30" s="19">
+        <v>4</v>
+      </c>
+      <c r="AB30" s="21"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE30" s="4">
+        <v>3</v>
+      </c>
+      <c r="AF30" s="21"/>
+      <c r="AG30" s="4">
+        <v>4</v>
+      </c>
+      <c r="AH30" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="21"/>
+      <c r="AK30" s="4">
+        <v>3</v>
+      </c>
+      <c r="AL30" s="4">
+        <v>2</v>
+      </c>
+      <c r="AM30" s="3"/>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="21"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="4">
+        <v>4</v>
+      </c>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="21"/>
+      <c r="AG31" s="3"/>
+      <c r="AH31" s="4">
+        <v>3</v>
+      </c>
+      <c r="AI31" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ31" s="21"/>
+      <c r="AK31" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL31" s="3"/>
+      <c r="AM31" s="3"/>
+    </row>
+    <row r="33" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X33">
+        <v>1</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X34">
+        <v>2</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X35">
+        <v>3</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH35" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X36">
+        <v>4</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH36" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="Y38" s="4">
+        <v>4</v>
+      </c>
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="20"/>
+      <c r="AB38" s="21"/>
+      <c r="AC38" s="3"/>
+      <c r="AD38" s="4">
+        <v>3</v>
+      </c>
+      <c r="AE38" s="4">
+        <v>4</v>
+      </c>
+      <c r="AF38" s="21"/>
+      <c r="AG38" s="3"/>
+      <c r="AH38" s="3"/>
+      <c r="AI38" s="3"/>
+      <c r="AJ38" s="21"/>
+      <c r="AK38" s="3"/>
+      <c r="AL38" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM38" s="3"/>
+    </row>
+    <row r="39" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="Y39" s="19">
+        <v>3</v>
+      </c>
+      <c r="Z39" s="19">
+        <v>2</v>
+      </c>
+      <c r="AA39" s="19">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="21"/>
+      <c r="AC39" s="3"/>
+      <c r="AD39" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE39" s="3"/>
+      <c r="AF39" s="21"/>
+      <c r="AG39" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH39" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI39" s="4">
+        <v>3</v>
+      </c>
+      <c r="AJ39" s="21"/>
+      <c r="AK39" s="3"/>
+      <c r="AL39" s="4">
+        <v>2</v>
+      </c>
+      <c r="AM39" s="3"/>
+    </row>
+    <row r="40" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="21"/>
+      <c r="AC40" s="3"/>
+      <c r="AD40" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE40" s="3"/>
+      <c r="AF40" s="21"/>
+      <c r="AG40" s="3"/>
+      <c r="AH40" s="3"/>
+      <c r="AI40" s="4">
+        <v>4</v>
+      </c>
+      <c r="AJ40" s="21"/>
+      <c r="AK40" s="4">
+        <v>4</v>
+      </c>
+      <c r="AL40" s="4">
+        <v>3</v>
+      </c>
+      <c r="AM40" s="3"/>
+    </row>
+    <row r="42" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X42">
+        <v>1</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH42" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X43">
+        <v>2</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH43" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X44">
+        <v>3</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH44" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X45">
+        <v>4</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH45" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="Y47" s="3"/>
+      <c r="Z47" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA47" s="19">
+        <v>4</v>
+      </c>
+      <c r="AB47" s="21"/>
+      <c r="AC47" s="3"/>
+      <c r="AD47" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE47" s="3"/>
+      <c r="AF47" s="21"/>
+      <c r="AG47" s="3"/>
+      <c r="AH47" s="3"/>
+      <c r="AI47" s="3"/>
+      <c r="AJ47" s="21"/>
+      <c r="AK47" s="3"/>
+      <c r="AL47" s="4">
+        <v>4</v>
+      </c>
+      <c r="AM47" s="3"/>
+    </row>
+    <row r="48" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="Y48" s="19">
+        <v>1</v>
+      </c>
+      <c r="Z48" s="19">
+        <v>2</v>
+      </c>
+      <c r="AA48" s="20"/>
+      <c r="AB48" s="21"/>
+      <c r="AC48" s="3"/>
+      <c r="AD48" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE48" s="4">
+        <v>3</v>
+      </c>
+      <c r="AF48" s="21"/>
+      <c r="AG48" s="3"/>
+      <c r="AH48" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI48" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ48" s="21"/>
+      <c r="AK48" s="3"/>
+      <c r="AL48" s="4">
+        <v>3</v>
+      </c>
+      <c r="AM48" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="Y49" s="3"/>
+      <c r="Z49" s="3"/>
+      <c r="AA49" s="3"/>
+      <c r="AB49" s="21"/>
+      <c r="AC49" s="3"/>
+      <c r="AD49" s="3"/>
+      <c r="AE49" s="4">
+        <v>4</v>
+      </c>
+      <c r="AF49" s="21"/>
+      <c r="AG49" s="4">
+        <v>4</v>
+      </c>
+      <c r="AH49" s="4">
+        <v>3</v>
+      </c>
+      <c r="AI49" s="3"/>
+      <c r="AJ49" s="21"/>
+      <c r="AK49" s="3"/>
+      <c r="AL49" s="3"/>
+      <c r="AM49" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X51">
+        <v>1</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH51" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL51" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X52">
+        <v>2</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD52" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH52" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X53">
+        <v>3</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD53" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH53" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X54">
+        <v>4</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD54" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH54" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="4">
+        <v>4</v>
+      </c>
+      <c r="AA56" s="20"/>
+      <c r="AB56" s="21"/>
+      <c r="AC56" s="3"/>
+      <c r="AD56" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE56" s="3"/>
+      <c r="AF56" s="21"/>
+      <c r="AG56" s="3"/>
+      <c r="AH56" s="3"/>
+      <c r="AI56" s="3"/>
+      <c r="AJ56" s="21"/>
+      <c r="AK56" s="3"/>
+      <c r="AL56" s="4">
+        <v>3</v>
+      </c>
+      <c r="AM56" s="3"/>
+    </row>
+    <row r="57" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="Y57" s="19">
+        <v>1</v>
+      </c>
+      <c r="Z57" s="19">
+        <v>2</v>
+      </c>
+      <c r="AA57" s="19">
+        <v>3</v>
+      </c>
+      <c r="AB57" s="21"/>
+      <c r="AC57" s="3"/>
+      <c r="AD57" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE57" s="4">
+        <v>4</v>
+      </c>
+      <c r="AF57" s="21"/>
+      <c r="AG57" s="4">
+        <v>3</v>
+      </c>
+      <c r="AH57" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI57" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ57" s="21"/>
+      <c r="AK57" s="4">
+        <v>4</v>
+      </c>
+      <c r="AL57" s="4">
+        <v>2</v>
+      </c>
+      <c r="AM57" s="3"/>
+    </row>
+    <row r="58" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="Y58" s="3"/>
+      <c r="Z58" s="3"/>
+      <c r="AA58" s="3"/>
+      <c r="AB58" s="21"/>
+      <c r="AC58" s="3"/>
+      <c r="AD58" s="4">
+        <v>3</v>
+      </c>
+      <c r="AE58" s="3"/>
+      <c r="AF58" s="21"/>
+      <c r="AG58" s="3"/>
+      <c r="AH58" s="4">
+        <v>4</v>
+      </c>
+      <c r="AI58" s="3"/>
+      <c r="AJ58" s="21"/>
+      <c r="AK58" s="3"/>
+      <c r="AL58" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM58" s="3"/>
+    </row>
+    <row r="60" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X60">
+        <v>1</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD60" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH60" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X61">
+        <v>2</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD61" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH61" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X62">
+        <v>3</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD62" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH62" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="24:39" x14ac:dyDescent="0.25">
+      <c r="X63">
+        <v>4</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD63" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH63" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL63" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BigHomeWork5 - can rotate and merge
</commit_message>
<xml_diff>
--- a/BigHomeWork5/Matrica.xlsx
+++ b/BigHomeWork5/Matrica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C_Sharp\GitHub\BigHomeWork5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6962DD-6FAF-49D1-8AF7-B1BD86771123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF85335-1774-428E-BFC9-50BB518A5086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="2610" windowWidth="20835" windowHeight="11385" xr2:uid="{2711DD60-25E4-4D42-9756-2F171D3D35B7}"/>
+    <workbookView xWindow="10035" yWindow="495" windowWidth="21600" windowHeight="11385" xr2:uid="{2711DD60-25E4-4D42-9756-2F171D3D35B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Lapas1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="25">
   <si>
     <t>(0;  24)</t>
   </si>
@@ -45,12 +45,6 @@
     <t>(0; 0)</t>
   </si>
   <si>
-    <t>(1; -1)</t>
-  </si>
-  <si>
-    <t>(1; 1)</t>
-  </si>
-  <si>
     <t>(-1; +1)</t>
   </si>
   <si>
@@ -66,9 +60,6 @@
     <t>(+2; 0)</t>
   </si>
   <si>
-    <t>(+1; +2)</t>
-  </si>
-  <si>
     <t>(-2; 0)</t>
   </si>
   <si>
@@ -106,6 +97,9 @@
   </si>
   <si>
     <t>(1; 0)</t>
+  </si>
+  <si>
+    <t>(1; +1)</t>
   </si>
 </sst>
 </file>
@@ -579,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C258D8-6C34-4A58-8345-2F6CC5536FF0}">
   <dimension ref="A1:AM63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AL3" sqref="AL3"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AL8" sqref="AL8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,8 +660,12 @@
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
+      <c r="AK2" s="4">
+        <v>4</v>
+      </c>
+      <c r="AL2" s="4">
+        <v>3</v>
+      </c>
       <c r="AM2" s="1"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
@@ -707,11 +705,15 @@
         <v>2</v>
       </c>
       <c r="AE3" s="1"/>
-      <c r="AG3" s="4"/>
+      <c r="AG3" s="4">
+        <v>3</v>
+      </c>
       <c r="AH3" s="4">
         <v>2</v>
       </c>
-      <c r="AI3" s="4"/>
+      <c r="AI3" s="4">
+        <v>1</v>
+      </c>
       <c r="AK3" s="1"/>
       <c r="AL3" s="4">
         <v>2</v>
@@ -753,11 +755,15 @@
       <c r="AE4" s="4">
         <v>4</v>
       </c>
-      <c r="AG4" s="4"/>
+      <c r="AG4" s="4">
+        <v>4</v>
+      </c>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
       <c r="AK4" s="1"/>
-      <c r="AL4" s="4"/>
+      <c r="AL4" s="4">
+        <v>1</v>
+      </c>
       <c r="AM4" s="1"/>
     </row>
     <row r="5" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
@@ -821,16 +827,16 @@
         <v>1</v>
       </c>
       <c r="Z6" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="AD6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AH6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="AL6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
@@ -905,16 +911,16 @@
         <v>3</v>
       </c>
       <c r="Z8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="AD8" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="AH8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AL8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
@@ -946,16 +952,16 @@
         <v>4</v>
       </c>
       <c r="Z9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AD9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="AH9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="AL9" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
@@ -1217,16 +1223,16 @@
         <v>1</v>
       </c>
       <c r="Z15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL15" t="s">
         <v>16</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>18</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
@@ -1301,16 +1307,16 @@
         <v>3</v>
       </c>
       <c r="Z17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AD17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AH17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AL17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
@@ -1342,16 +1348,16 @@
         <v>4</v>
       </c>
       <c r="Z18" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL18" t="s">
         <v>12</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>14</v>
-      </c>
-      <c r="AL18" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
@@ -1580,16 +1586,16 @@
         <v>1</v>
       </c>
       <c r="Z24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="AD24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="AH24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="AL24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
@@ -1674,16 +1680,16 @@
         <v>3</v>
       </c>
       <c r="Z26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AD26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AH26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AL26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
@@ -1691,16 +1697,16 @@
         <v>4</v>
       </c>
       <c r="Z27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AD27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AH27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AL27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
@@ -1794,13 +1800,13 @@
         <v>4</v>
       </c>
       <c r="AD33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AH33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AL33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="24:39" x14ac:dyDescent="0.25">
@@ -1825,16 +1831,16 @@
         <v>3</v>
       </c>
       <c r="Z35" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AD35" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AH35" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="AL35" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="24:39" x14ac:dyDescent="0.25">
@@ -1842,16 +1848,16 @@
         <v>4</v>
       </c>
       <c r="Z36" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AD36" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AH36" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AL36" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="24:39" x14ac:dyDescent="0.25">
@@ -1942,16 +1948,16 @@
         <v>1</v>
       </c>
       <c r="Z42" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="AD42" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AH42" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AL42" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="24:39" x14ac:dyDescent="0.25">
@@ -1976,16 +1982,16 @@
         <v>3</v>
       </c>
       <c r="Z44" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AD44" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AH44" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AL44" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="24:39" x14ac:dyDescent="0.25">
@@ -1993,16 +1999,16 @@
         <v>4</v>
       </c>
       <c r="Z45" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AD45" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AH45" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AL45" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="24:39" x14ac:dyDescent="0.25">
@@ -2024,11 +2030,11 @@
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
       <c r="AJ47" s="21"/>
-      <c r="AK47" s="3"/>
-      <c r="AL47" s="4">
-        <v>4</v>
-      </c>
-      <c r="AM47" s="3"/>
+      <c r="AK47" s="4">
+        <v>4</v>
+      </c>
+      <c r="AL47" s="3"/>
+      <c r="AM47" s="1"/>
     </row>
     <row r="48" spans="24:39" x14ac:dyDescent="0.25">
       <c r="Y48" s="19">
@@ -2055,13 +2061,13 @@
         <v>1</v>
       </c>
       <c r="AJ48" s="21"/>
-      <c r="AK48" s="3"/>
+      <c r="AK48" s="4">
+        <v>3</v>
+      </c>
       <c r="AL48" s="4">
-        <v>3</v>
-      </c>
-      <c r="AM48" s="4">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AM48" s="1"/>
     </row>
     <row r="49" spans="24:39" x14ac:dyDescent="0.25">
       <c r="Y49" s="3"/>
@@ -2083,26 +2089,26 @@
       <c r="AI49" s="3"/>
       <c r="AJ49" s="21"/>
       <c r="AK49" s="3"/>
-      <c r="AL49" s="3"/>
-      <c r="AM49" s="4">
-        <v>1</v>
-      </c>
+      <c r="AL49" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM49" s="1"/>
     </row>
     <row r="51" spans="24:39" x14ac:dyDescent="0.25">
       <c r="X51">
         <v>1</v>
       </c>
       <c r="Z51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="AD51" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AH51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AL51" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="24:39" x14ac:dyDescent="0.25">
@@ -2127,16 +2133,16 @@
         <v>3</v>
       </c>
       <c r="Z53" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AD53" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AH53" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AL53" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="24:39" x14ac:dyDescent="0.25">
@@ -2144,16 +2150,16 @@
         <v>4</v>
       </c>
       <c r="Z54" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AD54" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AH54" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="AL54" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="24:39" x14ac:dyDescent="0.25">
@@ -2244,16 +2250,16 @@
         <v>1</v>
       </c>
       <c r="Z60" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD60" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH60" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL60" t="s">
         <v>16</v>
-      </c>
-      <c r="AD60" t="s">
-        <v>18</v>
-      </c>
-      <c r="AH60" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL60" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="61" spans="24:39" x14ac:dyDescent="0.25">
@@ -2278,16 +2284,16 @@
         <v>3</v>
       </c>
       <c r="Z62" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AD62" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AH62" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AL62" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="24:39" x14ac:dyDescent="0.25">
@@ -2295,16 +2301,16 @@
         <v>4</v>
       </c>
       <c r="Z63" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AD63" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AH63" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AL63" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tetris - in progress (adding Timer)
</commit_message>
<xml_diff>
--- a/BigHomeWork5/Matrica.xlsx
+++ b/BigHomeWork5/Matrica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C_Sharp\GitHub\BigHomeWork5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF85335-1774-428E-BFC9-50BB518A5086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A68C97C-86ED-4B02-947B-7CD739657991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10035" yWindow="495" windowWidth="21600" windowHeight="11385" xr2:uid="{2711DD60-25E4-4D42-9756-2F171D3D35B7}"/>
+    <workbookView xWindow="5490" yWindow="765" windowWidth="21600" windowHeight="11385" xr2:uid="{2711DD60-25E4-4D42-9756-2F171D3D35B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Lapas1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="24">
   <si>
     <t>(0;  24)</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>(1; 0)</t>
-  </si>
-  <si>
-    <t>(1; +1)</t>
   </si>
 </sst>
 </file>
@@ -177,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -200,37 +197,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -247,9 +218,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -257,6 +225,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
@@ -573,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C258D8-6C34-4A58-8345-2F6CC5536FF0}">
   <dimension ref="A1:AM63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AL8" sqref="AL8"/>
+    <sheetView tabSelected="1" topLeftCell="P22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD34" sqref="AD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +619,7 @@
       </c>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="19">
+      <c r="AA2" s="16">
         <v>4</v>
       </c>
       <c r="AC2" s="1"/>
@@ -691,13 +661,13 @@
       <c r="R3" s="7">
         <v>1</v>
       </c>
-      <c r="Y3" s="19">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="19">
-        <v>2</v>
-      </c>
-      <c r="AA3" s="19">
+      <c r="Y3" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="16">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="16">
         <v>3</v>
       </c>
       <c r="AC3" s="1"/>
@@ -743,8 +713,10 @@
       <c r="R4" s="7">
         <v>1</v>
       </c>
-      <c r="T4" s="5"/>
-      <c r="U4" s="16"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="20"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
@@ -791,12 +763,10 @@
       <c r="R5" s="7">
         <v>1</v>
       </c>
-      <c r="T5" s="17"/>
-      <c r="U5" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="V5" s="18"/>
-      <c r="W5" s="4"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
     </row>
     <row r="6" spans="1:39" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
@@ -821,8 +791,10 @@
       <c r="R6" s="7">
         <v>1</v>
       </c>
-      <c r="T6" s="5"/>
-      <c r="U6" s="16"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
       <c r="X6">
         <v>1</v>
       </c>
@@ -864,8 +836,10 @@
       <c r="R7" s="7">
         <v>1</v>
       </c>
-      <c r="T7" s="5"/>
-      <c r="U7" s="16"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
       <c r="X7">
         <v>2</v>
       </c>
@@ -1040,7 +1014,7 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
-      <c r="AA11" s="20"/>
+      <c r="AA11" s="17"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="4">
@@ -1088,13 +1062,13 @@
       <c r="X12" s="4">
         <v>1</v>
       </c>
-      <c r="Y12" s="19">
-        <v>2</v>
-      </c>
-      <c r="Z12" s="19">
-        <v>3</v>
-      </c>
-      <c r="AA12" s="19">
+      <c r="Y12" s="16">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="16">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="16">
         <v>4</v>
       </c>
       <c r="AB12" s="1"/>
@@ -1413,10 +1387,10 @@
       <c r="Z20" s="4">
         <v>1</v>
       </c>
-      <c r="AA20" s="19">
-        <v>4</v>
-      </c>
-      <c r="AB20" s="21"/>
+      <c r="AA20" s="16">
+        <v>4</v>
+      </c>
+      <c r="AB20" s="18"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="4">
         <v>1</v>
@@ -1424,7 +1398,7 @@
       <c r="AE20" s="4">
         <v>4</v>
       </c>
-      <c r="AF20" s="21"/>
+      <c r="AF20" s="18"/>
       <c r="AG20" s="3"/>
       <c r="AH20" s="4">
         <v>1</v>
@@ -1432,7 +1406,7 @@
       <c r="AI20" s="4">
         <v>4</v>
       </c>
-      <c r="AJ20" s="21"/>
+      <c r="AJ20" s="18"/>
       <c r="AK20" s="3"/>
       <c r="AL20" s="4">
         <v>1</v>
@@ -1464,14 +1438,14 @@
       <c r="R21" s="7">
         <v>1</v>
       </c>
-      <c r="Y21" s="20"/>
-      <c r="Z21" s="19">
-        <v>2</v>
-      </c>
-      <c r="AA21" s="19">
-        <v>3</v>
-      </c>
-      <c r="AB21" s="21"/>
+      <c r="Y21" s="17"/>
+      <c r="Z21" s="16">
+        <v>2</v>
+      </c>
+      <c r="AA21" s="16">
+        <v>3</v>
+      </c>
+      <c r="AB21" s="18"/>
       <c r="AC21" s="3"/>
       <c r="AD21" s="4">
         <v>2</v>
@@ -1479,7 +1453,7 @@
       <c r="AE21" s="4">
         <v>3</v>
       </c>
-      <c r="AF21" s="21"/>
+      <c r="AF21" s="18"/>
       <c r="AG21" s="3"/>
       <c r="AH21" s="4">
         <v>2</v>
@@ -1487,7 +1461,7 @@
       <c r="AI21" s="4">
         <v>3</v>
       </c>
-      <c r="AJ21" s="21"/>
+      <c r="AJ21" s="18"/>
       <c r="AK21" s="3"/>
       <c r="AL21" s="4">
         <v>2</v>
@@ -1522,15 +1496,15 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
-      <c r="AB22" s="21"/>
+      <c r="AB22" s="18"/>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
       <c r="AE22" s="3"/>
-      <c r="AF22" s="21"/>
+      <c r="AF22" s="18"/>
       <c r="AG22" s="3"/>
       <c r="AH22" s="3"/>
       <c r="AI22" s="3"/>
-      <c r="AJ22" s="21"/>
+      <c r="AJ22" s="18"/>
       <c r="AK22" s="3"/>
       <c r="AL22" s="3"/>
       <c r="AM22" s="3"/>
@@ -1716,18 +1690,18 @@
       <c r="Z29" s="4">
         <v>3</v>
       </c>
-      <c r="AA29" s="20"/>
-      <c r="AB29" s="21"/>
+      <c r="AA29" s="17"/>
+      <c r="AB29" s="18"/>
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
       <c r="AE29" s="4">
         <v>1</v>
       </c>
-      <c r="AF29" s="21"/>
+      <c r="AF29" s="18"/>
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
       <c r="AI29" s="3"/>
-      <c r="AJ29" s="21"/>
+      <c r="AJ29" s="18"/>
       <c r="AK29" s="3"/>
       <c r="AL29" s="4">
         <v>4</v>
@@ -1735,14 +1709,14 @@
       <c r="AM29" s="3"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="Y30" s="20"/>
-      <c r="Z30" s="19">
-        <v>2</v>
-      </c>
-      <c r="AA30" s="19">
-        <v>4</v>
-      </c>
-      <c r="AB30" s="21"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="16">
+        <v>2</v>
+      </c>
+      <c r="AA30" s="16">
+        <v>4</v>
+      </c>
+      <c r="AB30" s="18"/>
       <c r="AC30" s="3"/>
       <c r="AD30" s="4">
         <v>2</v>
@@ -1750,7 +1724,7 @@
       <c r="AE30" s="4">
         <v>3</v>
       </c>
-      <c r="AF30" s="21"/>
+      <c r="AF30" s="18"/>
       <c r="AG30" s="4">
         <v>4</v>
       </c>
@@ -1758,7 +1732,7 @@
         <v>2</v>
       </c>
       <c r="AI30" s="3"/>
-      <c r="AJ30" s="21"/>
+      <c r="AJ30" s="18"/>
       <c r="AK30" s="4">
         <v>3</v>
       </c>
@@ -1771,13 +1745,13 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
       <c r="AA31" s="3"/>
-      <c r="AB31" s="21"/>
+      <c r="AB31" s="18"/>
       <c r="AC31" s="3"/>
       <c r="AD31" s="4">
         <v>4</v>
       </c>
       <c r="AE31" s="3"/>
-      <c r="AF31" s="21"/>
+      <c r="AF31" s="18"/>
       <c r="AG31" s="3"/>
       <c r="AH31" s="4">
         <v>3</v>
@@ -1785,7 +1759,7 @@
       <c r="AI31" s="4">
         <v>1</v>
       </c>
-      <c r="AJ31" s="21"/>
+      <c r="AJ31" s="18"/>
       <c r="AK31" s="4">
         <v>1</v>
       </c>
@@ -1803,7 +1777,7 @@
         <v>9</v>
       </c>
       <c r="AH33" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AL33" t="s">
         <v>6</v>
@@ -1831,13 +1805,13 @@
         <v>3</v>
       </c>
       <c r="Z35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AD35" t="s">
         <v>14</v>
       </c>
       <c r="AH35" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="AL35" t="s">
         <v>20</v>
@@ -1865,8 +1839,8 @@
         <v>4</v>
       </c>
       <c r="Z38" s="3"/>
-      <c r="AA38" s="20"/>
-      <c r="AB38" s="21"/>
+      <c r="AA38" s="17"/>
+      <c r="AB38" s="18"/>
       <c r="AC38" s="3"/>
       <c r="AD38" s="4">
         <v>3</v>
@@ -1874,11 +1848,11 @@
       <c r="AE38" s="4">
         <v>4</v>
       </c>
-      <c r="AF38" s="21"/>
+      <c r="AF38" s="18"/>
       <c r="AG38" s="3"/>
       <c r="AH38" s="3"/>
       <c r="AI38" s="3"/>
-      <c r="AJ38" s="21"/>
+      <c r="AJ38" s="18"/>
       <c r="AK38" s="3"/>
       <c r="AL38" s="4">
         <v>1</v>
@@ -1886,22 +1860,22 @@
       <c r="AM38" s="3"/>
     </row>
     <row r="39" spans="24:39" x14ac:dyDescent="0.25">
-      <c r="Y39" s="19">
-        <v>3</v>
-      </c>
-      <c r="Z39" s="19">
-        <v>2</v>
-      </c>
-      <c r="AA39" s="19">
-        <v>1</v>
-      </c>
-      <c r="AB39" s="21"/>
+      <c r="Y39" s="16">
+        <v>3</v>
+      </c>
+      <c r="Z39" s="16">
+        <v>2</v>
+      </c>
+      <c r="AA39" s="16">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="18"/>
       <c r="AC39" s="3"/>
       <c r="AD39" s="4">
         <v>2</v>
       </c>
       <c r="AE39" s="3"/>
-      <c r="AF39" s="21"/>
+      <c r="AF39" s="18"/>
       <c r="AG39" s="4">
         <v>1</v>
       </c>
@@ -1911,7 +1885,7 @@
       <c r="AI39" s="4">
         <v>3</v>
       </c>
-      <c r="AJ39" s="21"/>
+      <c r="AJ39" s="18"/>
       <c r="AK39" s="3"/>
       <c r="AL39" s="4">
         <v>2</v>
@@ -1922,19 +1896,19 @@
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
       <c r="AA40" s="3"/>
-      <c r="AB40" s="21"/>
+      <c r="AB40" s="18"/>
       <c r="AC40" s="3"/>
       <c r="AD40" s="4">
         <v>1</v>
       </c>
       <c r="AE40" s="3"/>
-      <c r="AF40" s="21"/>
+      <c r="AF40" s="18"/>
       <c r="AG40" s="3"/>
       <c r="AH40" s="3"/>
       <c r="AI40" s="4">
         <v>4</v>
       </c>
-      <c r="AJ40" s="21"/>
+      <c r="AJ40" s="18"/>
       <c r="AK40" s="4">
         <v>4</v>
       </c>
@@ -2016,20 +1990,20 @@
       <c r="Z47" s="4">
         <v>3</v>
       </c>
-      <c r="AA47" s="19">
-        <v>4</v>
-      </c>
-      <c r="AB47" s="21"/>
+      <c r="AA47" s="16">
+        <v>4</v>
+      </c>
+      <c r="AB47" s="18"/>
       <c r="AC47" s="3"/>
       <c r="AD47" s="4">
         <v>1</v>
       </c>
       <c r="AE47" s="3"/>
-      <c r="AF47" s="21"/>
+      <c r="AF47" s="18"/>
       <c r="AG47" s="3"/>
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
-      <c r="AJ47" s="21"/>
+      <c r="AJ47" s="18"/>
       <c r="AK47" s="4">
         <v>4</v>
       </c>
@@ -2037,14 +2011,14 @@
       <c r="AM47" s="1"/>
     </row>
     <row r="48" spans="24:39" x14ac:dyDescent="0.25">
-      <c r="Y48" s="19">
-        <v>1</v>
-      </c>
-      <c r="Z48" s="19">
-        <v>2</v>
-      </c>
-      <c r="AA48" s="20"/>
-      <c r="AB48" s="21"/>
+      <c r="Y48" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z48" s="16">
+        <v>2</v>
+      </c>
+      <c r="AA48" s="17"/>
+      <c r="AB48" s="18"/>
       <c r="AC48" s="3"/>
       <c r="AD48" s="4">
         <v>2</v>
@@ -2052,7 +2026,7 @@
       <c r="AE48" s="4">
         <v>3</v>
       </c>
-      <c r="AF48" s="21"/>
+      <c r="AF48" s="18"/>
       <c r="AG48" s="3"/>
       <c r="AH48" s="4">
         <v>2</v>
@@ -2060,7 +2034,7 @@
       <c r="AI48" s="4">
         <v>1</v>
       </c>
-      <c r="AJ48" s="21"/>
+      <c r="AJ48" s="18"/>
       <c r="AK48" s="4">
         <v>3</v>
       </c>
@@ -2073,13 +2047,13 @@
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
       <c r="AA49" s="3"/>
-      <c r="AB49" s="21"/>
+      <c r="AB49" s="18"/>
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
       <c r="AE49" s="4">
         <v>4</v>
       </c>
-      <c r="AF49" s="21"/>
+      <c r="AF49" s="18"/>
       <c r="AG49" s="4">
         <v>4</v>
       </c>
@@ -2087,7 +2061,7 @@
         <v>3</v>
       </c>
       <c r="AI49" s="3"/>
-      <c r="AJ49" s="21"/>
+      <c r="AJ49" s="18"/>
       <c r="AK49" s="3"/>
       <c r="AL49" s="4">
         <v>1</v>
@@ -2167,18 +2141,18 @@
       <c r="Z56" s="4">
         <v>4</v>
       </c>
-      <c r="AA56" s="20"/>
-      <c r="AB56" s="21"/>
+      <c r="AA56" s="17"/>
+      <c r="AB56" s="18"/>
       <c r="AC56" s="3"/>
       <c r="AD56" s="4">
         <v>1</v>
       </c>
       <c r="AE56" s="3"/>
-      <c r="AF56" s="21"/>
+      <c r="AF56" s="18"/>
       <c r="AG56" s="3"/>
       <c r="AH56" s="3"/>
       <c r="AI56" s="3"/>
-      <c r="AJ56" s="21"/>
+      <c r="AJ56" s="18"/>
       <c r="AK56" s="3"/>
       <c r="AL56" s="4">
         <v>3</v>
@@ -2186,16 +2160,16 @@
       <c r="AM56" s="3"/>
     </row>
     <row r="57" spans="24:39" x14ac:dyDescent="0.25">
-      <c r="Y57" s="19">
-        <v>1</v>
-      </c>
-      <c r="Z57" s="19">
-        <v>2</v>
-      </c>
-      <c r="AA57" s="19">
-        <v>3</v>
-      </c>
-      <c r="AB57" s="21"/>
+      <c r="Y57" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z57" s="16">
+        <v>2</v>
+      </c>
+      <c r="AA57" s="16">
+        <v>3</v>
+      </c>
+      <c r="AB57" s="18"/>
       <c r="AC57" s="3"/>
       <c r="AD57" s="4">
         <v>2</v>
@@ -2203,7 +2177,7 @@
       <c r="AE57" s="4">
         <v>4</v>
       </c>
-      <c r="AF57" s="21"/>
+      <c r="AF57" s="18"/>
       <c r="AG57" s="4">
         <v>3</v>
       </c>
@@ -2213,7 +2187,7 @@
       <c r="AI57" s="4">
         <v>1</v>
       </c>
-      <c r="AJ57" s="21"/>
+      <c r="AJ57" s="18"/>
       <c r="AK57" s="4">
         <v>4</v>
       </c>
@@ -2226,19 +2200,19 @@
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
       <c r="AA58" s="3"/>
-      <c r="AB58" s="21"/>
+      <c r="AB58" s="18"/>
       <c r="AC58" s="3"/>
       <c r="AD58" s="4">
         <v>3</v>
       </c>
       <c r="AE58" s="3"/>
-      <c r="AF58" s="21"/>
+      <c r="AF58" s="18"/>
       <c r="AG58" s="3"/>
       <c r="AH58" s="4">
         <v>4</v>
       </c>
       <c r="AI58" s="3"/>
-      <c r="AJ58" s="21"/>
+      <c r="AJ58" s="18"/>
       <c r="AK58" s="3"/>
       <c r="AL58" s="4">
         <v>1</v>

</xml_diff>